<commit_message>
Refactoring and Fixing code
</commit_message>
<xml_diff>
--- a/baseCategorized.xlsx
+++ b/baseCategorized.xlsx
@@ -466,7 +466,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -516,10 +516,10 @@
         <v>1</v>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
         <v>1</v>
@@ -533,7 +533,7 @@
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
         <v>1</v>
@@ -547,7 +547,7 @@
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
@@ -614,13 +614,13 @@
         <v>0</v>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -656,7 +656,7 @@
         <v>1</v>
       </c>
       <c r="B16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
@@ -670,7 +670,7 @@
         <v>1</v>
       </c>
       <c r="B17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
@@ -687,7 +687,7 @@
         <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" t="n">
         <v>1</v>
@@ -698,7 +698,7 @@
         <v>1</v>
       </c>
       <c r="B19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
@@ -718,7 +718,7 @@
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -746,7 +746,7 @@
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
@@ -768,7 +768,7 @@
         <v>1</v>
       </c>
       <c r="B24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
@@ -785,7 +785,7 @@
         <v>0</v>
       </c>
       <c r="C25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25" t="n">
         <v>1</v>
@@ -799,7 +799,7 @@
         <v>0</v>
       </c>
       <c r="C26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26" t="n">
         <v>1</v>
@@ -844,18 +844,18 @@
         <v>1</v>
       </c>
       <c r="D29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B30" t="n">
         <v>0</v>
       </c>
       <c r="C30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D30" t="n">
         <v>0</v>
@@ -872,7 +872,7 @@
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
@@ -936,7 +936,7 @@
         <v>0</v>
       </c>
       <c r="B36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
@@ -964,10 +964,10 @@
         <v>0</v>
       </c>
       <c r="B38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D38" t="n">
         <v>0</v>
@@ -981,7 +981,7 @@
         <v>0</v>
       </c>
       <c r="C39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D39" t="n">
         <v>0</v>
@@ -1006,7 +1006,7 @@
         <v>0</v>
       </c>
       <c r="B41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
@@ -1104,10 +1104,10 @@
         <v>0</v>
       </c>
       <c r="B48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D48" t="n">
         <v>0</v>
@@ -1163,7 +1163,7 @@
         <v>0</v>
       </c>
       <c r="C52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D52" t="n">
         <v>0</v>
@@ -1191,7 +1191,7 @@
         <v>0</v>
       </c>
       <c r="C54" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D54" t="n">
         <v>0</v>
@@ -1205,7 +1205,7 @@
         <v>0</v>
       </c>
       <c r="C55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D55" t="n">
         <v>0</v>
@@ -1222,7 +1222,7 @@
         <v>1</v>
       </c>
       <c r="D56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57">
@@ -1261,10 +1261,10 @@
         <v>1</v>
       </c>
       <c r="C59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60">
@@ -1272,18 +1272,18 @@
         <v>0</v>
       </c>
       <c r="B60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C60" t="n">
         <v>0</v>
       </c>
       <c r="D60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B61" t="n">
         <v>0</v>
@@ -1297,13 +1297,13 @@
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B62" t="n">
         <v>0</v>
       </c>
       <c r="C62" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D62" t="n">
         <v>0</v>
@@ -1376,7 +1376,7 @@
         <v>1</v>
       </c>
       <c r="D67" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68">
@@ -1387,7 +1387,7 @@
         <v>1</v>
       </c>
       <c r="C68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D68" t="n">
         <v>0</v>
@@ -1418,7 +1418,7 @@
         <v>1</v>
       </c>
       <c r="D70" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71">
@@ -1440,10 +1440,10 @@
         <v>0</v>
       </c>
       <c r="B72" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C72" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D72" t="n">
         <v>0</v>
@@ -1474,12 +1474,12 @@
         <v>0</v>
       </c>
       <c r="D74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B75" t="n">
         <v>0</v>
@@ -1502,7 +1502,7 @@
         <v>1</v>
       </c>
       <c r="D76" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77">
@@ -1513,7 +1513,7 @@
         <v>0</v>
       </c>
       <c r="C77" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D77" t="n">
         <v>0</v>
@@ -1524,7 +1524,7 @@
         <v>0</v>
       </c>
       <c r="B78" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C78" t="n">
         <v>0</v>
@@ -1549,7 +1549,7 @@
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B80" t="n">
         <v>0</v>
@@ -1569,7 +1569,7 @@
         <v>0</v>
       </c>
       <c r="C81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D81" t="n">
         <v>0</v>
@@ -1586,7 +1586,7 @@
         <v>1</v>
       </c>
       <c r="D82" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83">
@@ -1628,7 +1628,7 @@
         <v>1</v>
       </c>
       <c r="D85" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86">
@@ -1642,7 +1642,7 @@
         <v>1</v>
       </c>
       <c r="D86" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87">
@@ -1667,10 +1667,10 @@
         <v>0</v>
       </c>
       <c r="C88" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D88" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89">
@@ -1681,10 +1681,10 @@
         <v>0</v>
       </c>
       <c r="C89" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D89" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90">
@@ -1695,15 +1695,15 @@
         <v>0</v>
       </c>
       <c r="C90" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D90" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B91" t="n">
         <v>0</v>
@@ -1720,7 +1720,7 @@
         <v>0</v>
       </c>
       <c r="B92" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C92" t="n">
         <v>1</v>
@@ -1731,7 +1731,7 @@
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B93" t="n">
         <v>0</v>
@@ -1754,7 +1754,7 @@
         <v>1</v>
       </c>
       <c r="D94" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95">
@@ -1765,7 +1765,7 @@
         <v>0</v>
       </c>
       <c r="C95" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D95" t="n">
         <v>1</v>
@@ -1796,7 +1796,7 @@
         <v>0</v>
       </c>
       <c r="D97" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98">
@@ -1807,7 +1807,7 @@
         <v>0</v>
       </c>
       <c r="C98" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D98" t="n">
         <v>0</v>
@@ -1838,7 +1838,7 @@
         <v>0</v>
       </c>
       <c r="D100" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101">
@@ -1852,7 +1852,7 @@
         <v>1</v>
       </c>
       <c r="D101" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102">
@@ -1871,7 +1871,7 @@
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B103" t="n">
         <v>1</v>
@@ -1880,7 +1880,7 @@
         <v>0</v>
       </c>
       <c r="D103" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104">
@@ -1891,7 +1891,7 @@
         <v>1</v>
       </c>
       <c r="C104" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D104" t="n">
         <v>0</v>
@@ -1902,7 +1902,7 @@
         <v>0</v>
       </c>
       <c r="B105" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C105" t="n">
         <v>0</v>
@@ -1933,10 +1933,10 @@
         <v>0</v>
       </c>
       <c r="C107" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D107" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108">
@@ -1964,7 +1964,7 @@
         <v>0</v>
       </c>
       <c r="D109" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110">
@@ -1978,7 +1978,7 @@
         <v>0</v>
       </c>
       <c r="D110" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111">
@@ -1992,7 +1992,7 @@
         <v>1</v>
       </c>
       <c r="D111" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112">
@@ -2028,13 +2028,13 @@
         <v>0</v>
       </c>
       <c r="B114" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C114" t="n">
         <v>0</v>
       </c>
       <c r="D114" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115">
@@ -2048,7 +2048,7 @@
         <v>0</v>
       </c>
       <c r="D115" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116">
@@ -2104,7 +2104,7 @@
         <v>0</v>
       </c>
       <c r="D119" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="120">
@@ -2115,7 +2115,7 @@
         <v>0</v>
       </c>
       <c r="C120" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D120" t="n">
         <v>1</v>
@@ -2137,7 +2137,7 @@
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B122" t="n">
         <v>0</v>
@@ -2154,7 +2154,7 @@
         <v>0</v>
       </c>
       <c r="B123" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C123" t="n">
         <v>1</v>
@@ -2165,7 +2165,7 @@
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B124" t="n">
         <v>0</v>
@@ -2188,7 +2188,7 @@
         <v>0</v>
       </c>
       <c r="D125" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="126">
@@ -2238,13 +2238,13 @@
         <v>0</v>
       </c>
       <c r="B129" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C129" t="n">
         <v>0</v>
       </c>
       <c r="D129" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="130">
@@ -2252,13 +2252,13 @@
         <v>1</v>
       </c>
       <c r="B130" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C130" t="n">
         <v>1</v>
       </c>
       <c r="D130" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="131">
@@ -2300,7 +2300,7 @@
         <v>1</v>
       </c>
       <c r="D133" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="134">
@@ -2314,7 +2314,7 @@
         <v>0</v>
       </c>
       <c r="D134" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="135">
@@ -2339,7 +2339,7 @@
         <v>0</v>
       </c>
       <c r="C136" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D136" t="n">
         <v>0</v>
@@ -2350,13 +2350,13 @@
         <v>1</v>
       </c>
       <c r="B137" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C137" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D137" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="138">
@@ -2364,10 +2364,10 @@
         <v>1</v>
       </c>
       <c r="B138" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C138" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D138" t="n">
         <v>0</v>
@@ -2384,7 +2384,7 @@
         <v>0</v>
       </c>
       <c r="D139" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140">
@@ -2398,18 +2398,18 @@
         <v>1</v>
       </c>
       <c r="D140" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B141" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C141" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D141" t="n">
         <v>0</v>
@@ -2423,7 +2423,7 @@
         <v>0</v>
       </c>
       <c r="C142" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D142" t="n">
         <v>0</v>
@@ -2431,7 +2431,7 @@
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B143" t="n">
         <v>0</v>
@@ -2440,7 +2440,7 @@
         <v>1</v>
       </c>
       <c r="D143" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144">
@@ -2451,10 +2451,10 @@
         <v>1</v>
       </c>
       <c r="C144" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D144" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145">
@@ -2493,7 +2493,7 @@
         <v>0</v>
       </c>
       <c r="C147" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D147" t="n">
         <v>0</v>
@@ -2501,13 +2501,13 @@
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B148" t="n">
         <v>0</v>
       </c>
       <c r="C148" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D148" t="n">
         <v>0</v>
@@ -2529,7 +2529,7 @@
     </row>
     <row r="150">
       <c r="A150" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B150" t="n">
         <v>1</v>
@@ -2538,12 +2538,12 @@
         <v>0</v>
       </c>
       <c r="D150" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B151" t="n">
         <v>0</v>
@@ -2560,13 +2560,13 @@
         <v>0</v>
       </c>
       <c r="B152" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C152" t="n">
         <v>1</v>
       </c>
       <c r="D152" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="153">
@@ -2577,7 +2577,7 @@
         <v>0</v>
       </c>
       <c r="C153" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D153" t="n">
         <v>0</v>
@@ -2591,7 +2591,7 @@
         <v>0</v>
       </c>
       <c r="C154" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D154" t="n">
         <v>0</v>
@@ -2664,7 +2664,7 @@
         <v>0</v>
       </c>
       <c r="D159" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="160">
@@ -2678,7 +2678,7 @@
         <v>0</v>
       </c>
       <c r="D160" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="161">
@@ -2686,10 +2686,10 @@
         <v>1</v>
       </c>
       <c r="B161" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C161" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D161" t="n">
         <v>1</v>
@@ -2714,7 +2714,7 @@
         <v>1</v>
       </c>
       <c r="B163" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C163" t="n">
         <v>0</v>
@@ -2748,7 +2748,7 @@
         <v>0</v>
       </c>
       <c r="D165" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="166">
@@ -2762,7 +2762,7 @@
         <v>0</v>
       </c>
       <c r="D166" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="167">
@@ -2776,7 +2776,7 @@
         <v>0</v>
       </c>
       <c r="D167" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="168">
@@ -2812,7 +2812,7 @@
         <v>1</v>
       </c>
       <c r="B170" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C170" t="n">
         <v>1</v>
@@ -2837,7 +2837,7 @@
     </row>
     <row r="172">
       <c r="A172" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B172" t="n">
         <v>1</v>
@@ -2846,7 +2846,7 @@
         <v>0</v>
       </c>
       <c r="D172" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="173">
@@ -2874,7 +2874,7 @@
         <v>0</v>
       </c>
       <c r="D174" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="175">
@@ -2882,7 +2882,7 @@
         <v>1</v>
       </c>
       <c r="B175" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C175" t="n">
         <v>0</v>
@@ -2913,7 +2913,7 @@
         <v>1</v>
       </c>
       <c r="C177" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D177" t="n">
         <v>0</v>
@@ -2941,7 +2941,7 @@
         <v>0</v>
       </c>
       <c r="C179" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D179" t="n">
         <v>0</v>
@@ -2994,7 +2994,7 @@
         <v>0</v>
       </c>
       <c r="B183" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C183" t="n">
         <v>1</v>
@@ -3014,7 +3014,7 @@
         <v>1</v>
       </c>
       <c r="D184" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="185">
@@ -3025,10 +3025,10 @@
         <v>0</v>
       </c>
       <c r="C185" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D185" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="186">
@@ -3047,7 +3047,7 @@
     </row>
     <row r="187">
       <c r="A187" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B187" t="n">
         <v>1</v>
@@ -3078,7 +3078,7 @@
         <v>1</v>
       </c>
       <c r="B189" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C189" t="n">
         <v>0</v>
@@ -3098,7 +3098,7 @@
         <v>1</v>
       </c>
       <c r="D190" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="191">
@@ -3106,7 +3106,7 @@
         <v>1</v>
       </c>
       <c r="B191" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C191" t="n">
         <v>0</v>
@@ -3126,7 +3126,7 @@
         <v>0</v>
       </c>
       <c r="D192" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="193">
@@ -3137,7 +3137,7 @@
         <v>1</v>
       </c>
       <c r="C193" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D193" t="n">
         <v>0</v>
@@ -3151,7 +3151,7 @@
         <v>0</v>
       </c>
       <c r="C194" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D194" t="n">
         <v>0</v>
@@ -3176,7 +3176,7 @@
         <v>1</v>
       </c>
       <c r="B196" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C196" t="n">
         <v>1</v>
@@ -3201,7 +3201,7 @@
     </row>
     <row r="198">
       <c r="A198" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B198" t="n">
         <v>0</v>
@@ -3218,13 +3218,13 @@
         <v>1</v>
       </c>
       <c r="B199" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C199" t="n">
         <v>0</v>
       </c>
       <c r="D199" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="200">
@@ -3235,10 +3235,10 @@
         <v>0</v>
       </c>
       <c r="C200" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D200" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="201">
@@ -3249,10 +3249,10 @@
         <v>0</v>
       </c>
       <c r="C201" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D201" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="202">
@@ -3305,7 +3305,7 @@
         <v>1</v>
       </c>
       <c r="C205" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D205" t="n">
         <v>0</v>
@@ -3313,7 +3313,7 @@
     </row>
     <row r="206">
       <c r="A206" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B206" t="n">
         <v>0</v>
@@ -3322,7 +3322,7 @@
         <v>0</v>
       </c>
       <c r="D206" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="207">
@@ -3375,7 +3375,7 @@
         <v>1</v>
       </c>
       <c r="C210" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D210" t="n">
         <v>0</v>
@@ -3386,13 +3386,13 @@
         <v>1</v>
       </c>
       <c r="B211" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C211" t="n">
         <v>1</v>
       </c>
       <c r="D211" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="212">
@@ -3417,10 +3417,10 @@
         <v>1</v>
       </c>
       <c r="C213" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D213" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="214">
@@ -3428,7 +3428,7 @@
         <v>0</v>
       </c>
       <c r="B214" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C214" t="n">
         <v>1</v>
@@ -3456,10 +3456,10 @@
         <v>0</v>
       </c>
       <c r="B216" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C216" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D216" t="n">
         <v>0</v>
@@ -3473,10 +3473,10 @@
         <v>1</v>
       </c>
       <c r="C217" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D217" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="218">
@@ -3529,10 +3529,10 @@
         <v>0</v>
       </c>
       <c r="C221" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D221" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="222">
@@ -3540,7 +3540,7 @@
         <v>1</v>
       </c>
       <c r="B222" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C222" t="n">
         <v>1</v>
@@ -3574,7 +3574,7 @@
         <v>1</v>
       </c>
       <c r="D224" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="225">
@@ -3585,7 +3585,7 @@
         <v>1</v>
       </c>
       <c r="C225" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D225" t="n">
         <v>0</v>
@@ -3610,7 +3610,7 @@
         <v>1</v>
       </c>
       <c r="B227" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C227" t="n">
         <v>1</v>
@@ -3624,10 +3624,10 @@
         <v>0</v>
       </c>
       <c r="B228" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C228" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D228" t="n">
         <v>0</v>
@@ -3635,7 +3635,7 @@
     </row>
     <row r="229">
       <c r="A229" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B229" t="n">
         <v>0</v>
@@ -3655,7 +3655,7 @@
         <v>1</v>
       </c>
       <c r="C230" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D230" t="n">
         <v>0</v>
@@ -3666,7 +3666,7 @@
         <v>0</v>
       </c>
       <c r="B231" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C231" t="n">
         <v>1</v>
@@ -3711,7 +3711,7 @@
         <v>1</v>
       </c>
       <c r="C234" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D234" t="n">
         <v>0</v>
@@ -3719,7 +3719,7 @@
     </row>
     <row r="235">
       <c r="A235" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B235" t="n">
         <v>1</v>
@@ -3728,7 +3728,7 @@
         <v>0</v>
       </c>
       <c r="D235" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="236">
@@ -3784,7 +3784,7 @@
         <v>1</v>
       </c>
       <c r="D239" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="240">
@@ -3820,7 +3820,7 @@
         <v>1</v>
       </c>
       <c r="B242" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C242" t="n">
         <v>0</v>
@@ -3837,10 +3837,10 @@
         <v>0</v>
       </c>
       <c r="C243" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D243" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="244">
@@ -3854,7 +3854,7 @@
         <v>1</v>
       </c>
       <c r="D244" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="245">
@@ -3868,7 +3868,7 @@
         <v>0</v>
       </c>
       <c r="D245" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="246">
@@ -3890,7 +3890,7 @@
         <v>1</v>
       </c>
       <c r="B247" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C247" t="n">
         <v>0</v>
@@ -3932,7 +3932,7 @@
         <v>1</v>
       </c>
       <c r="B250" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C250" t="n">
         <v>0</v>
@@ -3980,18 +3980,18 @@
         <v>0</v>
       </c>
       <c r="D253" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B254" t="n">
         <v>0</v>
       </c>
       <c r="C254" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D254" t="n">
         <v>0</v>
@@ -4008,7 +4008,7 @@
         <v>1</v>
       </c>
       <c r="D255" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="256">
@@ -4022,12 +4022,12 @@
         <v>0</v>
       </c>
       <c r="D256" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B257" t="n">
         <v>0</v>
@@ -4069,13 +4069,13 @@
     </row>
     <row r="260">
       <c r="A260" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B260" t="n">
         <v>0</v>
       </c>
       <c r="C260" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D260" t="n">
         <v>0</v>
@@ -4092,12 +4092,12 @@
         <v>1</v>
       </c>
       <c r="D261" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B262" t="n">
         <v>0</v>
@@ -4156,7 +4156,7 @@
         <v>1</v>
       </c>
       <c r="B266" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C266" t="n">
         <v>0</v>
@@ -4184,13 +4184,13 @@
         <v>1</v>
       </c>
       <c r="B268" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C268" t="n">
         <v>0</v>
       </c>
       <c r="D268" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="269">
@@ -4240,10 +4240,10 @@
         <v>1</v>
       </c>
       <c r="B272" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C272" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D272" t="n">
         <v>0</v>
@@ -4257,7 +4257,7 @@
         <v>1</v>
       </c>
       <c r="C273" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D273" t="n">
         <v>0</v>
@@ -4285,10 +4285,10 @@
         <v>0</v>
       </c>
       <c r="C275" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D275" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="276">
@@ -4299,7 +4299,7 @@
         <v>1</v>
       </c>
       <c r="C276" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D276" t="n">
         <v>0</v>
@@ -4307,7 +4307,7 @@
     </row>
     <row r="277">
       <c r="A277" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B277" t="n">
         <v>1</v>
@@ -4352,13 +4352,13 @@
         <v>0</v>
       </c>
       <c r="B280" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C280" t="n">
         <v>1</v>
       </c>
       <c r="D280" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="281">
@@ -4366,7 +4366,7 @@
         <v>1</v>
       </c>
       <c r="B281" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C281" t="n">
         <v>1</v>
@@ -4383,7 +4383,7 @@
         <v>1</v>
       </c>
       <c r="C282" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D282" t="n">
         <v>1</v>
@@ -4439,15 +4439,15 @@
         <v>1</v>
       </c>
       <c r="C286" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D286" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B287" t="n">
         <v>1</v>
@@ -4484,7 +4484,7 @@
         <v>1</v>
       </c>
       <c r="D289" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="290">
@@ -4503,13 +4503,13 @@
     </row>
     <row r="291">
       <c r="A291" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B291" t="n">
         <v>1</v>
       </c>
       <c r="C291" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D291" t="n">
         <v>0</v>
@@ -4520,7 +4520,7 @@
         <v>0</v>
       </c>
       <c r="B292" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C292" t="n">
         <v>0</v>
@@ -4531,13 +4531,13 @@
     </row>
     <row r="293">
       <c r="A293" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B293" t="n">
         <v>1</v>
       </c>
       <c r="C293" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D293" t="n">
         <v>0</v>
@@ -4548,10 +4548,10 @@
         <v>0</v>
       </c>
       <c r="B294" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C294" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D294" t="n">
         <v>0</v>
@@ -4604,7 +4604,7 @@
         <v>0</v>
       </c>
       <c r="B298" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C298" t="n">
         <v>0</v>
@@ -4624,7 +4624,7 @@
         <v>1</v>
       </c>
       <c r="D299" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="300">
@@ -4635,7 +4635,7 @@
         <v>1</v>
       </c>
       <c r="C300" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D300" t="n">
         <v>0</v>
@@ -4643,7 +4643,7 @@
     </row>
     <row r="301">
       <c r="A301" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B301" t="n">
         <v>0</v>
@@ -4671,7 +4671,7 @@
     </row>
     <row r="303">
       <c r="A303" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B303" t="n">
         <v>0</v>
@@ -4680,7 +4680,7 @@
         <v>0</v>
       </c>
       <c r="D303" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="304">
@@ -4694,7 +4694,7 @@
         <v>0</v>
       </c>
       <c r="D304" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="305">
@@ -4702,13 +4702,13 @@
         <v>1</v>
       </c>
       <c r="B305" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C305" t="n">
         <v>0</v>
       </c>
       <c r="D305" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="306">
@@ -4716,7 +4716,7 @@
         <v>0</v>
       </c>
       <c r="B306" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C306" t="n">
         <v>0</v>
@@ -4733,7 +4733,7 @@
         <v>0</v>
       </c>
       <c r="C307" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D307" t="n">
         <v>0</v>
@@ -4741,13 +4741,13 @@
     </row>
     <row r="308">
       <c r="A308" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B308" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C308" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D308" t="n">
         <v>0</v>
@@ -4755,7 +4755,7 @@
     </row>
     <row r="309">
       <c r="A309" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B309" t="n">
         <v>1</v>
@@ -4775,10 +4775,10 @@
         <v>0</v>
       </c>
       <c r="C310" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D310" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="311">
@@ -4792,7 +4792,7 @@
         <v>1</v>
       </c>
       <c r="D311" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="312">
@@ -4834,7 +4834,7 @@
         <v>1</v>
       </c>
       <c r="D314" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="315">
@@ -4848,7 +4848,7 @@
         <v>0</v>
       </c>
       <c r="D315" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="316">
@@ -4881,7 +4881,7 @@
     </row>
     <row r="318">
       <c r="A318" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B318" t="n">
         <v>1</v>
@@ -4898,7 +4898,7 @@
         <v>1</v>
       </c>
       <c r="B319" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C319" t="n">
         <v>1</v>
@@ -4909,7 +4909,7 @@
     </row>
     <row r="320">
       <c r="A320" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B320" t="n">
         <v>0</v>
@@ -4918,7 +4918,7 @@
         <v>1</v>
       </c>
       <c r="D320" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="321">
@@ -4926,10 +4926,10 @@
         <v>1</v>
       </c>
       <c r="B321" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C321" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D321" t="n">
         <v>0</v>
@@ -4960,7 +4960,7 @@
         <v>0</v>
       </c>
       <c r="D323" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="324">
@@ -4968,7 +4968,7 @@
         <v>0</v>
       </c>
       <c r="B324" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C324" t="n">
         <v>0</v>
@@ -4985,10 +4985,10 @@
         <v>1</v>
       </c>
       <c r="C325" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D325" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="326">
@@ -4999,7 +4999,7 @@
         <v>1</v>
       </c>
       <c r="C326" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D326" t="n">
         <v>0</v>
@@ -5035,7 +5035,7 @@
     </row>
     <row r="329">
       <c r="A329" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B329" t="n">
         <v>0</v>
@@ -5063,7 +5063,7 @@
     </row>
     <row r="331">
       <c r="A331" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B331" t="n">
         <v>0</v>
@@ -5105,13 +5105,13 @@
     </row>
     <row r="334">
       <c r="A334" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B334" t="n">
         <v>0</v>
       </c>
       <c r="C334" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D334" t="n">
         <v>0</v>
@@ -5139,10 +5139,10 @@
         <v>0</v>
       </c>
       <c r="C336" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D336" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="337">
@@ -5153,7 +5153,7 @@
         <v>0</v>
       </c>
       <c r="C337" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D337" t="n">
         <v>0</v>
@@ -5178,10 +5178,10 @@
         <v>0</v>
       </c>
       <c r="B339" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C339" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D339" t="n">
         <v>0</v>
@@ -5192,7 +5192,7 @@
         <v>1</v>
       </c>
       <c r="B340" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C340" t="n">
         <v>1</v>
@@ -5209,7 +5209,7 @@
         <v>1</v>
       </c>
       <c r="C341" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D341" t="n">
         <v>1</v>
@@ -5318,13 +5318,13 @@
         <v>1</v>
       </c>
       <c r="B349" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C349" t="n">
         <v>0</v>
       </c>
       <c r="D349" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="350">
@@ -5371,10 +5371,10 @@
     </row>
     <row r="353">
       <c r="A353" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B353" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C353" t="n">
         <v>1</v>
@@ -5419,7 +5419,7 @@
         <v>0</v>
       </c>
       <c r="C356" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D356" t="n">
         <v>1</v>
@@ -5427,7 +5427,7 @@
     </row>
     <row r="357">
       <c r="A357" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B357" t="n">
         <v>0</v>
@@ -5441,7 +5441,7 @@
     </row>
     <row r="358">
       <c r="A358" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B358" t="n">
         <v>0</v>
@@ -5461,7 +5461,7 @@
         <v>0</v>
       </c>
       <c r="C359" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D359" t="n">
         <v>0</v>
@@ -5472,10 +5472,10 @@
         <v>1</v>
       </c>
       <c r="B360" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C360" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D360" t="n">
         <v>1</v>
@@ -5500,7 +5500,7 @@
         <v>0</v>
       </c>
       <c r="B362" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C362" t="n">
         <v>0</v>
@@ -5548,7 +5548,7 @@
         <v>1</v>
       </c>
       <c r="D365" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="366">
@@ -5562,7 +5562,7 @@
         <v>1</v>
       </c>
       <c r="D366" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="367">
@@ -5573,7 +5573,7 @@
         <v>0</v>
       </c>
       <c r="C367" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D367" t="n">
         <v>1</v>
@@ -5584,7 +5584,7 @@
         <v>0</v>
       </c>
       <c r="B368" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C368" t="n">
         <v>0</v>
@@ -5626,7 +5626,7 @@
         <v>0</v>
       </c>
       <c r="B371" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C371" t="n">
         <v>1</v>
@@ -5674,7 +5674,7 @@
         <v>1</v>
       </c>
       <c r="D374" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="375">
@@ -5688,7 +5688,7 @@
         <v>0</v>
       </c>
       <c r="D375" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="376">
@@ -5699,7 +5699,7 @@
         <v>0</v>
       </c>
       <c r="C376" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D376" t="n">
         <v>0</v>
@@ -5772,7 +5772,7 @@
         <v>1</v>
       </c>
       <c r="D381" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="382">
@@ -5783,7 +5783,7 @@
         <v>1</v>
       </c>
       <c r="C382" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D382" t="n">
         <v>0</v>
@@ -5805,7 +5805,7 @@
     </row>
     <row r="384">
       <c r="A384" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B384" t="n">
         <v>1</v>
@@ -5814,7 +5814,7 @@
         <v>0</v>
       </c>
       <c r="D384" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="385">
@@ -5825,7 +5825,7 @@
         <v>0</v>
       </c>
       <c r="C385" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D385" t="n">
         <v>1</v>
@@ -5853,7 +5853,7 @@
         <v>0</v>
       </c>
       <c r="C387" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D387" t="n">
         <v>0</v>
@@ -5867,7 +5867,7 @@
         <v>1</v>
       </c>
       <c r="C388" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D388" t="n">
         <v>0</v>
@@ -5937,10 +5937,10 @@
         <v>0</v>
       </c>
       <c r="C393" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D393" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="394">
@@ -5951,7 +5951,7 @@
         <v>0</v>
       </c>
       <c r="C394" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D394" t="n">
         <v>0</v>
@@ -5968,12 +5968,12 @@
         <v>1</v>
       </c>
       <c r="D395" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="396">
       <c r="A396" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B396" t="n">
         <v>0</v>
@@ -6004,7 +6004,7 @@
         <v>1</v>
       </c>
       <c r="B398" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C398" t="n">
         <v>1</v>
@@ -6015,7 +6015,7 @@
     </row>
     <row r="399">
       <c r="A399" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B399" t="n">
         <v>0</v>
@@ -6088,7 +6088,7 @@
         <v>1</v>
       </c>
       <c r="B404" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C404" t="n">
         <v>1</v>
@@ -6099,7 +6099,7 @@
     </row>
     <row r="405">
       <c r="A405" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B405" t="n">
         <v>0</v>
@@ -6158,7 +6158,7 @@
         <v>1</v>
       </c>
       <c r="B409" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C409" t="n">
         <v>0</v>
@@ -6214,13 +6214,13 @@
         <v>1</v>
       </c>
       <c r="B413" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C413" t="n">
         <v>0</v>
       </c>
       <c r="D413" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="414">
@@ -6234,7 +6234,7 @@
         <v>0</v>
       </c>
       <c r="D414" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="415">
@@ -6248,7 +6248,7 @@
         <v>1</v>
       </c>
       <c r="D415" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="416">
@@ -6256,7 +6256,7 @@
         <v>1</v>
       </c>
       <c r="B416" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C416" t="n">
         <v>0</v>
@@ -6276,7 +6276,7 @@
         <v>1</v>
       </c>
       <c r="D417" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="418">
@@ -6284,7 +6284,7 @@
         <v>0</v>
       </c>
       <c r="B418" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C418" t="n">
         <v>0</v>
@@ -6298,7 +6298,7 @@
         <v>1</v>
       </c>
       <c r="B419" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C419" t="n">
         <v>1</v>
@@ -6343,7 +6343,7 @@
         <v>1</v>
       </c>
       <c r="C422" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D422" t="n">
         <v>1</v>
@@ -6371,10 +6371,10 @@
         <v>0</v>
       </c>
       <c r="C424" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D424" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="425">
@@ -6388,7 +6388,7 @@
         <v>1</v>
       </c>
       <c r="D425" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="426">
@@ -6427,7 +6427,7 @@
         <v>0</v>
       </c>
       <c r="C428" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D428" t="n">
         <v>1</v>
@@ -6449,7 +6449,7 @@
     </row>
     <row r="430">
       <c r="A430" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B430" t="n">
         <v>0</v>
@@ -6469,10 +6469,10 @@
         <v>0</v>
       </c>
       <c r="C431" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D431" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="432">
@@ -6497,7 +6497,7 @@
         <v>1</v>
       </c>
       <c r="C433" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D433" t="n">
         <v>0</v>
@@ -6514,7 +6514,7 @@
         <v>1</v>
       </c>
       <c r="D434" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="435">
@@ -6528,7 +6528,7 @@
         <v>0</v>
       </c>
       <c r="D435" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="436">
@@ -6536,7 +6536,7 @@
         <v>0</v>
       </c>
       <c r="B436" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C436" t="n">
         <v>1</v>
@@ -6581,7 +6581,7 @@
         <v>0</v>
       </c>
       <c r="C439" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D439" t="n">
         <v>1</v>
@@ -6592,18 +6592,18 @@
         <v>0</v>
       </c>
       <c r="B440" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C440" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D440" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="441">
       <c r="A441" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B441" t="n">
         <v>0</v>
@@ -6612,7 +6612,7 @@
         <v>0</v>
       </c>
       <c r="D441" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="442">
@@ -6665,7 +6665,7 @@
         <v>1</v>
       </c>
       <c r="C445" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D445" t="n">
         <v>0</v>
@@ -6693,7 +6693,7 @@
         <v>1</v>
       </c>
       <c r="C447" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D447" t="n">
         <v>0</v>
@@ -6701,13 +6701,13 @@
     </row>
     <row r="448">
       <c r="A448" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B448" t="n">
         <v>1</v>
       </c>
       <c r="C448" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D448" t="n">
         <v>0</v>
@@ -6732,7 +6732,7 @@
         <v>0</v>
       </c>
       <c r="B450" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C450" t="n">
         <v>0</v>
@@ -6743,7 +6743,7 @@
     </row>
     <row r="451">
       <c r="A451" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B451" t="n">
         <v>0</v>
@@ -6780,7 +6780,7 @@
         <v>1</v>
       </c>
       <c r="D453" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="454">
@@ -6794,7 +6794,7 @@
         <v>1</v>
       </c>
       <c r="D454" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="455">
@@ -6869,7 +6869,7 @@
     </row>
     <row r="460">
       <c r="A460" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B460" t="n">
         <v>0</v>
@@ -6878,7 +6878,7 @@
         <v>0</v>
       </c>
       <c r="D460" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="461">
@@ -6903,7 +6903,7 @@
         <v>1</v>
       </c>
       <c r="C462" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D462" t="n">
         <v>0</v>
@@ -6911,10 +6911,10 @@
     </row>
     <row r="463">
       <c r="A463" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B463" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C463" t="n">
         <v>0</v>
@@ -6928,7 +6928,7 @@
         <v>1</v>
       </c>
       <c r="B464" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C464" t="n">
         <v>0</v>
@@ -6939,7 +6939,7 @@
     </row>
     <row r="465">
       <c r="A465" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B465" t="n">
         <v>1</v>
@@ -6981,13 +6981,13 @@
     </row>
     <row r="468">
       <c r="A468" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B468" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C468" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D468" t="n">
         <v>1</v>
@@ -7004,7 +7004,7 @@
         <v>1</v>
       </c>
       <c r="D469" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="470">
@@ -7032,15 +7032,15 @@
         <v>0</v>
       </c>
       <c r="D471" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="472">
       <c r="A472" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B472" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C472" t="n">
         <v>0</v>
@@ -7051,7 +7051,7 @@
     </row>
     <row r="473">
       <c r="A473" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B473" t="n">
         <v>0</v>
@@ -7065,7 +7065,7 @@
     </row>
     <row r="474">
       <c r="A474" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B474" t="n">
         <v>0</v>
@@ -7079,7 +7079,7 @@
     </row>
     <row r="475">
       <c r="A475" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B475" t="n">
         <v>1</v>
@@ -7107,7 +7107,7 @@
     </row>
     <row r="477">
       <c r="A477" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B477" t="n">
         <v>0</v>
@@ -7138,13 +7138,13 @@
         <v>1</v>
       </c>
       <c r="B479" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C479" t="n">
         <v>1</v>
       </c>
       <c r="D479" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="480">
@@ -7166,7 +7166,7 @@
         <v>0</v>
       </c>
       <c r="B481" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C481" t="n">
         <v>0</v>
@@ -7186,7 +7186,7 @@
         <v>1</v>
       </c>
       <c r="D482" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="483">
@@ -7242,15 +7242,15 @@
         <v>1</v>
       </c>
       <c r="D486" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="487">
       <c r="A487" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B487" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C487" t="n">
         <v>0</v>
@@ -7284,7 +7284,7 @@
         <v>0</v>
       </c>
       <c r="D489" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="490">
@@ -7303,7 +7303,7 @@
     </row>
     <row r="491">
       <c r="A491" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B491" t="n">
         <v>0</v>
@@ -7362,7 +7362,7 @@
         <v>1</v>
       </c>
       <c r="B495" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C495" t="n">
         <v>0</v>
@@ -7390,7 +7390,7 @@
         <v>0</v>
       </c>
       <c r="B497" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C497" t="n">
         <v>0</v>
@@ -7421,7 +7421,7 @@
         <v>0</v>
       </c>
       <c r="C499" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D499" t="n">
         <v>0</v>
@@ -7432,13 +7432,13 @@
         <v>0</v>
       </c>
       <c r="B500" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C500" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D500" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="501">
@@ -7480,7 +7480,7 @@
         <v>1</v>
       </c>
       <c r="D503" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="504">
@@ -7491,7 +7491,7 @@
         <v>1</v>
       </c>
       <c r="C504" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D504" t="n">
         <v>0</v>
@@ -7505,10 +7505,10 @@
         <v>0</v>
       </c>
       <c r="C505" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D505" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="506">
@@ -7544,7 +7544,7 @@
         <v>1</v>
       </c>
       <c r="B508" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C508" t="n">
         <v>0</v>
@@ -7555,7 +7555,7 @@
     </row>
     <row r="509">
       <c r="A509" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B509" t="n">
         <v>1</v>
@@ -7569,7 +7569,7 @@
     </row>
     <row r="510">
       <c r="A510" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B510" t="n">
         <v>1</v>
@@ -7578,7 +7578,7 @@
         <v>0</v>
       </c>
       <c r="D510" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="511">
@@ -7589,7 +7589,7 @@
         <v>1</v>
       </c>
       <c r="C511" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D511" t="n">
         <v>0</v>
@@ -7600,13 +7600,13 @@
         <v>0</v>
       </c>
       <c r="B512" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C512" t="n">
         <v>0</v>
       </c>
       <c r="D512" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="513">
@@ -7614,7 +7614,7 @@
         <v>0</v>
       </c>
       <c r="B513" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C513" t="n">
         <v>0</v>
@@ -7634,7 +7634,7 @@
         <v>0</v>
       </c>
       <c r="D514" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="515">
@@ -7642,7 +7642,7 @@
         <v>1</v>
       </c>
       <c r="B515" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C515" t="n">
         <v>0</v>
@@ -7662,7 +7662,7 @@
         <v>1</v>
       </c>
       <c r="D516" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="517">

</xml_diff>